<commit_message>
update lab notebook and TOC
</commit_message>
<xml_diff>
--- a/Nutrients/mbl_nuts112025/raw/MBL CHLA NOV 25.xlsx
+++ b/Nutrients/mbl_nuts112025/raw/MBL CHLA NOV 25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jadefiorilla/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookesienkiewicz/Documents/LabNotebook/Nutrients/mbl_nuts112025/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9236322-6129-7844-8D52-77A92977076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3144E06C-4875-C44C-AD90-F707F0B03934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{3D7F1DBA-A993-4EA7-9E5B-0DC7349DDDD7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18380" xr2:uid="{3D7F1DBA-A993-4EA7-9E5B-0DC7349DDDD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1001,7 +1001,8 @@
   <dimension ref="A2:S127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <pane ySplit="7" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3613,11 +3614,11 @@
         <v>76</v>
       </c>
       <c r="C55" s="11">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" si="8"/>
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="E55" s="11">
         <v>4.87</v>
@@ -3639,22 +3640,22 @@
       </c>
       <c r="J55" s="7">
         <f t="shared" si="12"/>
-        <v>0.20572971457696229</v>
+        <v>0.23144592889908255</v>
       </c>
       <c r="K55" s="7">
         <f t="shared" si="13"/>
-        <v>7.3285285423037694E-2</v>
+        <v>8.2445946100917405E-2</v>
       </c>
       <c r="L55" s="11">
         <v>1</v>
       </c>
       <c r="M55" s="14">
         <f t="shared" si="14"/>
-        <v>0.20572971457696229</v>
+        <v>0.23144592889908255</v>
       </c>
       <c r="N55" s="7">
         <f t="shared" si="15"/>
-        <v>7.3285285423037694E-2</v>
+        <v>8.2445946100917405E-2</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -4081,11 +4082,11 @@
         <v>85</v>
       </c>
       <c r="C64" s="11">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="D64" s="2">
         <f t="shared" si="16"/>
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="E64" s="11">
         <v>0.29399999999999998</v>
@@ -4107,22 +4108,22 @@
       </c>
       <c r="J64" s="7">
         <f t="shared" si="20"/>
-        <v>1.1092339449541284E-2</v>
+        <v>1.6638509174311929E-2</v>
       </c>
       <c r="K64" s="7">
         <f t="shared" si="21"/>
-        <v>7.1986438837920493E-3</v>
+        <v>1.0797965825688073E-2</v>
       </c>
       <c r="L64" s="11">
         <v>1</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" si="22"/>
-        <v>1.1092339449541284E-2</v>
+        <v>1.6638509174311929E-2</v>
       </c>
       <c r="N64" s="7">
         <f t="shared" si="23"/>
-        <v>7.1986438837920493E-3</v>
+        <v>1.0797965825688073E-2</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
@@ -4448,11 +4449,11 @@
         <v>94</v>
       </c>
       <c r="C71" s="11">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="D71" s="2">
         <f t="shared" si="16"/>
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="E71" s="11">
         <v>1.1399999999999999</v>
@@ -4474,22 +4475,22 @@
       </c>
       <c r="J71" s="7">
         <f t="shared" si="20"/>
-        <v>3.7448496432212028E-2</v>
+        <v>5.6172744648318042E-2</v>
       </c>
       <c r="K71" s="7">
         <f t="shared" si="21"/>
-        <v>3.9538975790010193E-2</v>
+        <v>5.9308463685015286E-2</v>
       </c>
       <c r="L71" s="11">
         <v>1</v>
       </c>
       <c r="M71" s="14">
         <f t="shared" si="22"/>
-        <v>3.7448496432212028E-2</v>
+        <v>5.6172744648318042E-2</v>
       </c>
       <c r="N71" s="7">
         <f t="shared" si="23"/>
-        <v>3.9538975790010193E-2</v>
+        <v>5.9308463685015286E-2</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
@@ -5491,11 +5492,11 @@
         <v>114</v>
       </c>
       <c r="C91" s="11">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D91" s="2">
         <f t="shared" si="16"/>
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="E91" s="11">
         <v>18.3</v>
@@ -5517,22 +5518,22 @@
       </c>
       <c r="J91" s="7">
         <f t="shared" si="20"/>
-        <v>0.70156676860346601</v>
+        <v>0.84188012232415921</v>
       </c>
       <c r="K91" s="7">
         <f t="shared" si="21"/>
-        <v>0.42482712028542291</v>
+        <v>0.50979254434250754</v>
       </c>
       <c r="L91" s="11">
         <v>1</v>
       </c>
       <c r="M91" s="14">
         <f t="shared" si="22"/>
-        <v>0.70156676860346601</v>
+        <v>0.84188012232415921</v>
       </c>
       <c r="N91" s="7">
         <f t="shared" si="23"/>
-        <v>0.42482712028542291</v>
+        <v>0.50979254434250754</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -6014,11 +6015,11 @@
         <v>125</v>
       </c>
       <c r="C101" s="11">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D101" s="2">
         <f t="shared" si="24"/>
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="E101" s="11">
         <v>18.600000000000001</v>
@@ -6040,22 +6041,22 @@
       </c>
       <c r="J101" s="7">
         <f t="shared" si="28"/>
-        <v>0.54039602446483193</v>
+        <v>0.64847522935779833</v>
       </c>
       <c r="K101" s="7">
         <f t="shared" si="29"/>
-        <v>0.79267564220183473</v>
+        <v>0.95121077064220172</v>
       </c>
       <c r="L101" s="11">
         <v>1</v>
       </c>
       <c r="M101" s="14">
         <f t="shared" si="30"/>
-        <v>0.54039602446483193</v>
+        <v>0.64847522935779833</v>
       </c>
       <c r="N101" s="7">
         <f t="shared" si="31"/>
-        <v>0.79267564220183473</v>
+        <v>0.95121077064220172</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>